<commit_message>
Scripting SCD0330 and fixing SCD0331
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0330 - Report staging activity.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0330 - Report staging activity.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099B0F27-330B-4AB1-9C30-05D553023FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FA480E0-1229-4A1A-B866-7D1A82C92C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3645" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCD0330" sheetId="2" r:id="rId1"/>
@@ -160,10 +160,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF333333"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,14 +217,14 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -534,7 +535,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,97 +562,98 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="P1" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="Q1" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="13" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="114.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="14" t="s">
         <v>23</v>
       </c>
       <c r="F2" s="5">
         <v>51162</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
       <c r="L2" s="5"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="7"/>
-      <c r="R2" s="7"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="14"/>
       <c r="S2" s="1"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">

</xml_diff>